<commit_message>
AB - Game Flow
</commit_message>
<xml_diff>
--- a/UE5Part2/ArenaBattle/GameData/ABCharacterStatTable.xlsx
+++ b/UE5Part2/ArenaBattle/GameData/ABCharacterStatTable.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UE5Part2\PreTest\ArenaBattle10pre\GameData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\UE5Part2\ArenaBattle\GameData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B6DBFFE-125E-4A66-AF5B-85CEEB9F49AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1A37F4-3253-4CB0-A52E-26CA7ADC6EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="1120" windowWidth="31540" windowHeight="17940" xr2:uid="{14535CBB-5647-4022-885E-3A0FC95BEC4B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14400" xr2:uid="{14535CBB-5647-4022-885E-3A0FC95BEC4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="2" r:id="rId1"/>
@@ -448,7 +448,7 @@
   <dimension ref="A2:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -486,7 +486,7 @@
         <v>100</v>
       </c>
       <c r="C3" s="1">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1">
         <v>40</v>
@@ -506,7 +506,7 @@
         <v>150</v>
       </c>
       <c r="C4" s="1">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="D4" s="1">
         <v>40</v>
@@ -526,7 +526,7 @@
         <v>200</v>
       </c>
       <c r="C5" s="1">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="D5" s="1">
         <v>40</v>
@@ -566,7 +566,7 @@
         <v>300</v>
       </c>
       <c r="C7" s="1">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="D7" s="1">
         <v>40</v>
@@ -586,7 +586,7 @@
         <v>350</v>
       </c>
       <c r="C8" s="1">
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="D8" s="1">
         <v>40</v>
@@ -606,7 +606,7 @@
         <v>400</v>
       </c>
       <c r="C9" s="1">
-        <v>220</v>
+        <v>280</v>
       </c>
       <c r="D9" s="1">
         <v>40</v>
@@ -626,7 +626,7 @@
         <v>450</v>
       </c>
       <c r="C10" s="1">
-        <v>240</v>
+        <v>320</v>
       </c>
       <c r="D10" s="1">
         <v>40</v>
@@ -646,7 +646,7 @@
         <v>500</v>
       </c>
       <c r="C11" s="1">
-        <v>260</v>
+        <v>360</v>
       </c>
       <c r="D11" s="1">
         <v>40</v>
@@ -666,7 +666,7 @@
         <v>550</v>
       </c>
       <c r="C12" s="1">
-        <v>280</v>
+        <v>400</v>
       </c>
       <c r="D12" s="1">
         <v>40</v>

</xml_diff>